<commit_message>
Deploying to gh-pages from  @ 73d3e014505b8798740169e0a25908d007e1c776 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/15.1.1.1.xlsx
+++ b/en/downloads/data-excel/15.1.1.1.xlsx
@@ -729,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -746,7 +746,7 @@
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25">
+    <row r="1" spans="1:12" ht="38.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -757,7 +757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
@@ -768,12 +768,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -807,8 +807,11 @@
       <c r="K4" s="13">
         <v>2019</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="13">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -842,8 +845,11 @@
       <c r="K5" s="19">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="19">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -877,8 +883,11 @@
       <c r="K6" s="20">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -912,8 +921,11 @@
       <c r="K7" s="20">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="20">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -947,8 +959,11 @@
       <c r="K8" s="20">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -982,8 +997,11 @@
       <c r="K9" s="20">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1017,8 +1035,11 @@
       <c r="K10" s="20">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1052,8 +1073,11 @@
       <c r="K11" s="20">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1">
+      <c r="L11" s="20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -1087,8 +1111,11 @@
       <c r="K12" s="21">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="34.5">
+      <c r="L12" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="34.5">
       <c r="A13" s="18" t="s">
         <v>32</v>
       </c>

</xml_diff>